<commit_message>
some more design and archive for projects
</commit_message>
<xml_diff>
--- a/public/evaluations/LKatmp.xlsx
+++ b/public/evaluations/LKatmp.xlsx
@@ -1011,6 +1011,177 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c t="inlineStr">
+        <is>
+          <t>Project A</t>
+        </is>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>Continuing</t>
+        </is>
+      </c>
+      <c>
+        <v>2022</v>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>January</t>
+        </is>
+      </c>
+      <c>
+        <v>120</v>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>Rome Dudley</t>
+        </is>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>RDu</t>
+        </is>
+      </c>
+      <c>
+        <v>23</v>
+      </c>
+      <c>
+        <v>2</v>
+      </c>
+      <c>
+        <v>21</v>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>Continuing</t>
+        </is>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c t="inlineStr">
+        <is>
+          <t>Project A</t>
+        </is>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>Continuing</t>
+        </is>
+      </c>
+      <c>
+        <v>2022</v>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>February</t>
+        </is>
+      </c>
+      <c>
+        <v>120</v>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>Rome Dudley</t>
+        </is>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>RDu</t>
+        </is>
+      </c>
+      <c>
+        <v>23</v>
+      </c>
+      <c>
+        <v>21</v>
+      </c>
+      <c>
+        <v>2</v>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>Continuing</t>
+        </is>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c t="inlineStr">
+        <is>
+          <t>Project B</t>
+        </is>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>Continuing</t>
+        </is>
+      </c>
+      <c>
+        <v>2022</v>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>February</t>
+        </is>
+      </c>
+      <c>
+        <v>234</v>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>Rome Dudley</t>
+        </is>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>RDu</t>
+        </is>
+      </c>
+      <c>
+        <v>23</v>
+      </c>
+      <c>
+        <v>13.5</v>
+      </c>
+      <c>
+        <v>9.5</v>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>Continuing</t>
+        </is>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>